<commit_message>
Adding changes after incorporating custom metrics for video events
</commit_message>
<xml_diff>
--- a/Files/InputRules/Rules.xlsx
+++ b/Files/InputRules/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahota\PycharmProjects\GA\Files\InputRules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1875E7CC-3B51-4EEE-AAF7-0B0B42C71B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB5DEE1-5ACC-4180-B6A1-F42D4377C7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="685" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="685" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="11" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="TAXONOMYSC" sheetId="4" r:id="rId4"/>
     <sheet name="TAXONOMY" sheetId="6" r:id="rId5"/>
     <sheet name="BIO" sheetId="9" r:id="rId6"/>
-    <sheet name="GENERALVIDEO" sheetId="13" r:id="rId7"/>
+    <sheet name="VIDEO" sheetId="13" r:id="rId7"/>
+    <sheet name="GENERALVIDEO" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="98">
   <si>
     <t>Parameter</t>
   </si>
@@ -223,13 +224,124 @@
   </si>
   <si>
     <t>healthdotcom-article Click</t>
+  </si>
+  <si>
+    <t>Video Player Metadata</t>
+  </si>
+  <si>
+    <t>Video Player Initialized</t>
+  </si>
+  <si>
+    <t>Video Playback Buffer Started</t>
+  </si>
+  <si>
+    <t>Video Player Options Interaction</t>
+  </si>
+  <si>
+    <t>Video Playback View Impression</t>
+  </si>
+  <si>
+    <t>Video Ad Started</t>
+  </si>
+  <si>
+    <t>Video Ad Player Shown</t>
+  </si>
+  <si>
+    <t>Video Ad Playing</t>
+  </si>
+  <si>
+    <t>Video Ad Viewable 2sec Req</t>
+  </si>
+  <si>
+    <t>Video Ad Completed</t>
+  </si>
+  <si>
+    <t>Video Content Started</t>
+  </si>
+  <si>
+    <t>Video Content Started 3sec</t>
+  </si>
+  <si>
+    <t>Video Playback Paused</t>
+  </si>
+  <si>
+    <t>Video Playback Resumed</t>
+  </si>
+  <si>
+    <t>cm1</t>
+  </si>
+  <si>
+    <t>cm3</t>
+  </si>
+  <si>
+    <t>cm4</t>
+  </si>
+  <si>
+    <t>cm5</t>
+  </si>
+  <si>
+    <t>cm6</t>
+  </si>
+  <si>
+    <t>cm7</t>
+  </si>
+  <si>
+    <t>cm8</t>
+  </si>
+  <si>
+    <t>cm12</t>
+  </si>
+  <si>
+    <t>cm13</t>
+  </si>
+  <si>
+    <t>cm14</t>
+  </si>
+  <si>
+    <t>cm15</t>
+  </si>
+  <si>
+    <t>cm16</t>
+  </si>
+  <si>
+    <t>cm38</t>
+  </si>
+  <si>
+    <t>cm39</t>
+  </si>
+  <si>
+    <t>cm40</t>
+  </si>
+  <si>
+    <t>cm41</t>
+  </si>
+  <si>
+    <t>cm45</t>
+  </si>
+  <si>
+    <t>cm46</t>
+  </si>
+  <si>
+    <t>cm47</t>
+  </si>
+  <si>
+    <t>cm48</t>
+  </si>
+  <si>
+    <t>cm49</t>
+  </si>
+  <si>
+    <t>cm61</t>
+  </si>
+  <si>
+    <t>cm37</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +408,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -318,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -359,6 +478,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -643,7 +778,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,22 +797,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2184,6 +2319,343 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082C6F02-958E-43CE-BA32-291E5C3A0801}">
   <dimension ref="A1:G35"/>
   <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="54.7109375" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5">
+        <v>100</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F60:F1048576 F18:F34 E1:E12 E15:E17" xr:uid="{54367D5A-6A99-43FC-B8D0-C6BC27A91867}">
+      <formula1>"int, str"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E60:E1048576 E18:E34 D1:D12 D15:D17" xr:uid="{25E71491-2583-4921-ACBC-91A8600DE64B}">
+      <formula1>"Data Type, Data Value, Data Format"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D35 F16 D60:D1048576 F4:F12 C1:C12 C15:C17" xr:uid="{13E2BA9D-5273-4236-8324-238986F0D4F0}">
+      <formula1>"R, O"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1C1B9A-8D80-4EEC-818B-3C60F465E48C}">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:G9"/>
     </sheetView>
@@ -2241,345 +2713,6 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5">
-        <v>100</v>
-      </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="2"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F60:F1048576 F18:F34 E1:E12 E15:E17" xr:uid="{54367D5A-6A99-43FC-B8D0-C6BC27A91867}">
-      <formula1>"int, str"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E60:E1048576 E18:E34 D1:D12 D15:D17" xr:uid="{25E71491-2583-4921-ACBC-91A8600DE64B}">
-      <formula1>"Data Type, Data Value, Data Format"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D35 F16 D60:D1048576 F4:F12 C1:C12 C15:C17" xr:uid="{13E2BA9D-5273-4236-8324-238986F0D4F0}">
-      <formula1>"R, O"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1C1B9A-8D80-4EEC-818B-3C60F465E48C}">
-  <dimension ref="A1:G35"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="54.7109375" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
-    <col min="12" max="12" width="29.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G2" s="5"/>
@@ -2834,10 +2967,2156 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FA1E3E-6FE2-4CAE-ABC3-D3B29BC2DDFD}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G352"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="37.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="19"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="B37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="19"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="B38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="20"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="B39" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="9"/>
+      <c r="G40" s="19"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="19"/>
+      <c r="B41" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="9"/>
+      <c r="G41" s="19"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
+      <c r="B42" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="20"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="B43" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="19"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="B45" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="9"/>
+      <c r="G45" s="19"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="B46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="20"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="B47" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="19"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
+      <c r="B49" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="9"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="19"/>
+      <c r="B50" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="20"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+      <c r="B51" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="8"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="8"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="8"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="8"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="8"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="8"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="8"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="8"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="8"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="8"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="8"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="8"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="8"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="8"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="8"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="8"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="8"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="8"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="8"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="8"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="8"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="8"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="8"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="8"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="8"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="8"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="8"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="8"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="8"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="8"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="8"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="8"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="8"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="8"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="8"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="8"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="8"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="8"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="8"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="8"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="8"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="8"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="8"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="8"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="8"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="8"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="8"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="8"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="8"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="8"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="8"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="8"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="8"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="8"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="8"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="8"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="8"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="8"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="8"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="8"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="8"/>
+      <c r="C121" s="5"/>
+      <c r="D121" s="5"/>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="8"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="8"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="8"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="8"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="8"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="8"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="8"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="8"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="8"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="8"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="8"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="8"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="8"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="8"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="8"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5"/>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="8"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="8"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="8"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5"/>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="8"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="8"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="5"/>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="8"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="5"/>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="8"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="8"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="8"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5"/>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="8"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="8"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="8"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="5"/>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="8"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="5"/>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="8"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="8"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="8"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="5"/>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="8"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="5"/>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="8"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5"/>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="8"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="8"/>
+      <c r="C162" s="5"/>
+      <c r="D162" s="5"/>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="8"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="5"/>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="8"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="8"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="5"/>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="8"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="5"/>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="8"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5"/>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="8"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="5"/>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="8"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="5"/>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="8"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="5"/>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="8"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="5"/>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="8"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="5"/>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="8"/>
+      <c r="C173" s="5"/>
+      <c r="D173" s="5"/>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174" s="8"/>
+      <c r="C174" s="5"/>
+      <c r="D174" s="5"/>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="8"/>
+      <c r="C175" s="5"/>
+      <c r="D175" s="5"/>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="8"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="5"/>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B177" s="8"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="8"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="5"/>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B182" s="8"/>
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B183" s="8"/>
+      <c r="C183" s="5"/>
+      <c r="D183" s="5"/>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B184" s="8"/>
+      <c r="C184" s="5"/>
+      <c r="D184" s="5"/>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B185" s="8"/>
+      <c r="C185" s="5"/>
+      <c r="D185" s="5"/>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B186" s="8"/>
+      <c r="C186" s="5"/>
+      <c r="D186" s="5"/>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B187" s="8"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="5"/>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B188" s="8"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="5"/>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B189" s="8"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="5"/>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B190" s="8"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="5"/>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B191" s="8"/>
+      <c r="C191" s="5"/>
+      <c r="D191" s="5"/>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B192" s="8"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="5"/>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B193" s="8"/>
+      <c r="C193" s="5"/>
+      <c r="D193" s="5"/>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B194" s="8"/>
+      <c r="C194" s="5"/>
+      <c r="D194" s="5"/>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195" s="8"/>
+      <c r="C195" s="5"/>
+      <c r="D195" s="5"/>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B196" s="8"/>
+      <c r="C196" s="5"/>
+      <c r="D196" s="5"/>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B197" s="8"/>
+      <c r="C197" s="5"/>
+      <c r="D197" s="5"/>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B198" s="8"/>
+      <c r="C198" s="5"/>
+      <c r="D198" s="5"/>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B199" s="8"/>
+      <c r="C199" s="5"/>
+      <c r="D199" s="5"/>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B200" s="8"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="5"/>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B201" s="8"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="5"/>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B202" s="8"/>
+      <c r="C202" s="5"/>
+      <c r="D202" s="5"/>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B206" s="8"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="5"/>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B207" s="8"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="5"/>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B208" s="8"/>
+      <c r="C208" s="5"/>
+      <c r="D208" s="5"/>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B209" s="8"/>
+      <c r="C209" s="5"/>
+      <c r="D209" s="5"/>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B210" s="8"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="5"/>
+    </row>
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B211" s="8"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="5"/>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B212" s="8"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="5"/>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B213" s="8"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="5"/>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B214" s="8"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="5"/>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B215" s="8"/>
+      <c r="C215" s="5"/>
+      <c r="D215" s="5"/>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B216" s="8"/>
+      <c r="C216" s="5"/>
+      <c r="D216" s="5"/>
+    </row>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B217" s="8"/>
+      <c r="C217" s="5"/>
+      <c r="D217" s="5"/>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B218" s="8"/>
+      <c r="C218" s="5"/>
+      <c r="D218" s="5"/>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B219" s="8"/>
+      <c r="C219" s="5"/>
+      <c r="D219" s="5"/>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B220" s="8"/>
+      <c r="C220" s="5"/>
+      <c r="D220" s="5"/>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B221" s="8"/>
+      <c r="C221" s="5"/>
+      <c r="D221" s="5"/>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B222" s="8"/>
+      <c r="C222" s="5"/>
+      <c r="D222" s="5"/>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B223" s="8"/>
+      <c r="C223" s="5"/>
+      <c r="D223" s="5"/>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B224" s="8"/>
+      <c r="C224" s="5"/>
+      <c r="D224" s="5"/>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B225" s="8"/>
+      <c r="C225" s="5"/>
+      <c r="D225" s="5"/>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B226" s="8"/>
+      <c r="C226" s="5"/>
+      <c r="D226" s="5"/>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B227" s="8"/>
+      <c r="C227" s="5"/>
+      <c r="D227" s="5"/>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B241" s="8"/>
+      <c r="C241" s="5"/>
+      <c r="D241" s="5"/>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B242" s="8"/>
+      <c r="C242" s="5"/>
+      <c r="D242" s="5"/>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B243" s="8"/>
+      <c r="C243" s="5"/>
+      <c r="D243" s="5"/>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B244" s="8"/>
+      <c r="C244" s="5"/>
+      <c r="D244" s="5"/>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B245" s="8"/>
+      <c r="C245" s="5"/>
+      <c r="D245" s="5"/>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B246" s="8"/>
+      <c r="C246" s="5"/>
+      <c r="D246" s="5"/>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B247" s="8"/>
+      <c r="C247" s="5"/>
+      <c r="D247" s="5"/>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B248" s="8"/>
+      <c r="C248" s="5"/>
+      <c r="D248" s="5"/>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B249" s="8"/>
+      <c r="C249" s="5"/>
+      <c r="D249" s="5"/>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B250" s="8"/>
+      <c r="C250" s="5"/>
+      <c r="D250" s="5"/>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B251" s="8"/>
+      <c r="C251" s="5"/>
+      <c r="D251" s="5"/>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B252" s="8"/>
+      <c r="C252" s="5"/>
+      <c r="D252" s="5"/>
+    </row>
+    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B263" s="8"/>
+      <c r="C263" s="5"/>
+      <c r="D263" s="5"/>
+    </row>
+    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B264" s="8"/>
+      <c r="C264" s="5"/>
+      <c r="D264" s="5"/>
+    </row>
+    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B265" s="8"/>
+      <c r="C265" s="5"/>
+      <c r="D265" s="5"/>
+    </row>
+    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B266" s="8"/>
+      <c r="C266" s="5"/>
+      <c r="D266" s="5"/>
+    </row>
+    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B267" s="8"/>
+      <c r="C267" s="5"/>
+      <c r="D267" s="5"/>
+    </row>
+    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B268" s="8"/>
+      <c r="C268" s="5"/>
+      <c r="D268" s="5"/>
+    </row>
+    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B269" s="8"/>
+      <c r="C269" s="5"/>
+      <c r="D269" s="5"/>
+    </row>
+    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B270" s="8"/>
+      <c r="C270" s="5"/>
+      <c r="D270" s="5"/>
+    </row>
+    <row r="271" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B271" s="8"/>
+      <c r="C271" s="5"/>
+      <c r="D271" s="5"/>
+    </row>
+    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B272" s="8"/>
+      <c r="C272" s="5"/>
+      <c r="D272" s="5"/>
+    </row>
+    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B273" s="8"/>
+      <c r="C273" s="5"/>
+      <c r="D273" s="5"/>
+    </row>
+    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B274" s="8"/>
+      <c r="C274" s="5"/>
+      <c r="D274" s="5"/>
+    </row>
+    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B275" s="8"/>
+      <c r="C275" s="5"/>
+      <c r="D275" s="5"/>
+    </row>
+    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B276" s="8"/>
+      <c r="C276" s="5"/>
+      <c r="D276" s="5"/>
+    </row>
+    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B277" s="8"/>
+      <c r="C277" s="5"/>
+      <c r="D277" s="5"/>
+    </row>
+    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B285" s="8"/>
+      <c r="C285" s="5"/>
+      <c r="D285" s="5"/>
+    </row>
+    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B286" s="8"/>
+      <c r="C286" s="5"/>
+      <c r="D286" s="5"/>
+    </row>
+    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B287" s="8"/>
+      <c r="C287" s="5"/>
+      <c r="D287" s="5"/>
+    </row>
+    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B288" s="8"/>
+      <c r="C288" s="5"/>
+      <c r="D288" s="5"/>
+    </row>
+    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B289" s="8"/>
+      <c r="C289" s="5"/>
+      <c r="D289" s="5"/>
+    </row>
+    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B290" s="8"/>
+      <c r="C290" s="5"/>
+      <c r="D290" s="5"/>
+    </row>
+    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B291" s="8"/>
+      <c r="C291" s="5"/>
+      <c r="D291" s="5"/>
+    </row>
+    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B292" s="8"/>
+      <c r="C292" s="5"/>
+      <c r="D292" s="5"/>
+    </row>
+    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B293" s="8"/>
+      <c r="C293" s="5"/>
+      <c r="D293" s="5"/>
+    </row>
+    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B294" s="8"/>
+      <c r="C294" s="5"/>
+      <c r="D294" s="5"/>
+    </row>
+    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B295" s="8"/>
+      <c r="C295" s="5"/>
+      <c r="D295" s="5"/>
+    </row>
+    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B296" s="8"/>
+      <c r="C296" s="5"/>
+      <c r="D296" s="5"/>
+    </row>
+    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B297" s="8"/>
+      <c r="C297" s="5"/>
+      <c r="D297" s="5"/>
+    </row>
+    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B298" s="8"/>
+      <c r="C298" s="5"/>
+      <c r="D298" s="5"/>
+    </row>
+    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B299" s="8"/>
+      <c r="C299" s="5"/>
+      <c r="D299" s="5"/>
+    </row>
+    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B300" s="8"/>
+      <c r="C300" s="5"/>
+      <c r="D300" s="5"/>
+    </row>
+    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B301" s="8"/>
+      <c r="C301" s="5"/>
+      <c r="D301" s="5"/>
+    </row>
+    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B302" s="8"/>
+      <c r="C302" s="5"/>
+      <c r="D302" s="5"/>
+    </row>
+    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B309" s="8"/>
+      <c r="C309" s="5"/>
+      <c r="D309" s="5"/>
+    </row>
+    <row r="310" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B310" s="8"/>
+      <c r="C310" s="5"/>
+      <c r="D310" s="5"/>
+    </row>
+    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B311" s="8"/>
+      <c r="C311" s="5"/>
+      <c r="D311" s="5"/>
+    </row>
+    <row r="312" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B312" s="8"/>
+      <c r="C312" s="5"/>
+      <c r="D312" s="5"/>
+    </row>
+    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B313" s="8"/>
+      <c r="C313" s="5"/>
+      <c r="D313" s="5"/>
+    </row>
+    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B314" s="8"/>
+      <c r="C314" s="5"/>
+      <c r="D314" s="5"/>
+    </row>
+    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B315" s="8"/>
+      <c r="C315" s="5"/>
+      <c r="D315" s="5"/>
+    </row>
+    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B316" s="8"/>
+      <c r="C316" s="5"/>
+      <c r="D316" s="5"/>
+    </row>
+    <row r="317" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B317" s="8"/>
+      <c r="C317" s="5"/>
+      <c r="D317" s="5"/>
+    </row>
+    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B318" s="8"/>
+      <c r="C318" s="5"/>
+      <c r="D318" s="5"/>
+    </row>
+    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B319" s="8"/>
+      <c r="C319" s="5"/>
+      <c r="D319" s="5"/>
+    </row>
+    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B320" s="8"/>
+      <c r="C320" s="5"/>
+      <c r="D320" s="5"/>
+    </row>
+    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B321" s="8"/>
+      <c r="C321" s="5"/>
+      <c r="D321" s="5"/>
+    </row>
+    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B322" s="8"/>
+      <c r="C322" s="5"/>
+      <c r="D322" s="5"/>
+    </row>
+    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B323" s="8"/>
+      <c r="C323" s="5"/>
+      <c r="D323" s="5"/>
+    </row>
+    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B324" s="8"/>
+      <c r="C324" s="5"/>
+      <c r="D324" s="5"/>
+    </row>
+    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B325" s="8"/>
+      <c r="C325" s="5"/>
+      <c r="D325" s="5"/>
+    </row>
+    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B326" s="8"/>
+      <c r="C326" s="5"/>
+      <c r="D326" s="5"/>
+    </row>
+    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B327" s="8"/>
+      <c r="C327" s="5"/>
+      <c r="D327" s="5"/>
+    </row>
+    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B331" s="8"/>
+      <c r="C331" s="5"/>
+      <c r="D331" s="5"/>
+    </row>
+    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B332" s="8"/>
+      <c r="C332" s="5"/>
+      <c r="D332" s="5"/>
+    </row>
+    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B333" s="8"/>
+      <c r="C333" s="5"/>
+      <c r="D333" s="5"/>
+    </row>
+    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B334" s="8"/>
+      <c r="C334" s="5"/>
+      <c r="D334" s="5"/>
+    </row>
+    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B335" s="8"/>
+      <c r="C335" s="5"/>
+      <c r="D335" s="5"/>
+    </row>
+    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B336" s="8"/>
+      <c r="C336" s="5"/>
+      <c r="D336" s="5"/>
+    </row>
+    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B337" s="8"/>
+      <c r="C337" s="5"/>
+      <c r="D337" s="5"/>
+    </row>
+    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B338" s="8"/>
+      <c r="C338" s="5"/>
+      <c r="D338" s="5"/>
+    </row>
+    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B339" s="8"/>
+      <c r="C339" s="5"/>
+      <c r="D339" s="5"/>
+    </row>
+    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B340" s="8"/>
+      <c r="C340" s="5"/>
+      <c r="D340" s="5"/>
+    </row>
+    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B341" s="8"/>
+      <c r="C341" s="5"/>
+      <c r="D341" s="5"/>
+    </row>
+    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B342" s="8"/>
+      <c r="C342" s="5"/>
+      <c r="D342" s="5"/>
+    </row>
+    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B343" s="8"/>
+      <c r="C343" s="5"/>
+      <c r="D343" s="5"/>
+    </row>
+    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B344" s="8"/>
+      <c r="C344" s="5"/>
+      <c r="D344" s="5"/>
+    </row>
+    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B345" s="8"/>
+      <c r="C345" s="5"/>
+      <c r="D345" s="5"/>
+    </row>
+    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B346" s="8"/>
+      <c r="C346" s="5"/>
+      <c r="D346" s="5"/>
+    </row>
+    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B347" s="8"/>
+      <c r="C347" s="5"/>
+      <c r="D347" s="5"/>
+    </row>
+    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B348" s="8"/>
+      <c r="C348" s="5"/>
+      <c r="D348" s="5"/>
+    </row>
+    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B349" s="8"/>
+      <c r="C349" s="5"/>
+      <c r="D349" s="5"/>
+    </row>
+    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B350" s="8"/>
+      <c r="C350" s="5"/>
+      <c r="D350" s="5"/>
+    </row>
+    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B351" s="8"/>
+      <c r="C351" s="5"/>
+      <c r="D351" s="5"/>
+    </row>
+    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B352" s="8"/>
+      <c r="C352" s="5"/>
+      <c r="D352" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10 F12:F14 F16:F21 D353:D1048576 C81:C102 C106:C127 C131:C152 C156:C177 F23:F28 C181:C202 C331:C352 C309:C327 C285:C302 C263:C277 C206:C227 C241:C252 F30:F35 F36:F38 C1:C35 F40:F42 F44:F46 F48:F50 C36:C51 C55:C77" xr:uid="{D20E6B53-167E-4CDB-BA93-C823778C9A7C}">
+      <formula1>"R, O"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E353:E1048576 D81:D102 D106:D127 D131:D152 D156:D177 D181:D202 D331:D352 D309:D327 D285:D302 D263:D277 D206:D227 D241:D252 D1:D35 D36:D51 D55:D77" xr:uid="{7A7BAD41-2491-4CEF-91D3-D55CC6FD232F}">
+      <formula1>"Data Type, Data Value, Data Format"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E10 E12:E14 E16:E21 E23:E28 E30:E35 F353:F1048576 E36:E38 E40:E42 E44:E46 E48:E50" xr:uid="{9EA68936-52D6-488C-B9A7-6F3DCE32D084}">
+      <formula1>"int, str"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609697A1-6682-4559-9A8A-347AAF7808BE}">
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,8 +5125,8 @@
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="54.85546875" customWidth="1"/>
+    <col min="7" max="7" width="34.5703125" customWidth="1"/>
     <col min="8" max="8" width="37.28515625" customWidth="1"/>
     <col min="9" max="9" width="22.28515625" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" customWidth="1"/>
@@ -2855,62 +5134,57 @@
     <col min="12" max="12" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -2918,182 +5192,289 @@
       <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="F4" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="A17" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="A18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="A19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="A20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="A21" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="A22" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="A23" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="A24" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
@@ -3123,13 +5504,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D60:D1048576 B16:B28 F6 F8:F10 E2:E4 B1:B4 C5:C11" xr:uid="{D20E6B53-167E-4CDB-BA93-C823778C9A7C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D60:D1048576 B1:B24 B28" xr:uid="{577A418F-30B1-44F9-84F2-9F4581BEA223}">
       <formula1>"R, O"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E60:E1048576 C16:C27 C1:C4 D5:D11" xr:uid="{7A7BAD41-2491-4CEF-91D3-D55CC6FD232F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E60:E1048576 C1:C24" xr:uid="{C3ADD4B5-8A40-49F3-9C4C-3ED7F6FC5D2B}">
       <formula1>"Data Type, Data Value, Data Format"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F60:F1048576 D16:D27 D1:D4 E5:E11" xr:uid="{9EA68936-52D6-488C-B9A7-6F3DCE32D084}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F60:F1048576 D1" xr:uid="{12E1024D-F867-41C5-8226-B26DCC3FCB53}">
       <formula1>"int, str"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>